<commit_message>
Fixed Major Printing Bug (prints / computes wrong values in options)
</commit_message>
<xml_diff>
--- a/Chi-Test__a1(1 2 ).csv__a2(0 1 ).csv_.xlsx
+++ b/Chi-Test__a1(1 2 ).csv__a2(0 1 ).csv_.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Candy\Documents\GitHub\OOTO Miner Python v2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7F6AE9-1F9A-498A-B662-796D71A6F441}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="936" yWindow="1920" windowWidth="22104" windowHeight="8580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1066,8 +1072,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1076,12 +1082,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1096,14 +1108,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1150,7 +1171,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1182,9 +1203,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1216,6 +1255,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1391,14 +1448,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10:L10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1406,7 +1465,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1414,7 +1473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1422,7 +1481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1469,7 +1528,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1477,7 +1536,7 @@
         <v>21</v>
       </c>
       <c r="C5">
-        <v>2.715097830567618</v>
+        <v>2.7150978305676179</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
@@ -1486,10 +1545,10 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G5">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" ref="G5:G36" si="0">IF(C:C&gt;F:F,1,0)</f>
         <v>0</v>
       </c>
       <c r="H5">
@@ -1517,7 +1576,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1525,7 +1584,7 @@
         <v>29</v>
       </c>
       <c r="C6">
-        <v>0.4811155202508678</v>
+        <v>0.48111552025086779</v>
       </c>
       <c r="D6" t="s">
         <v>30</v>
@@ -1534,10 +1593,10 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G6">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H6">
@@ -1565,7 +1624,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1582,10 +1641,10 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G7">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H7">
@@ -1613,7 +1672,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1621,7 +1680,7 @@
         <v>40</v>
       </c>
       <c r="C8">
-        <v>0.7765032539214347</v>
+        <v>0.77650325392143471</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
@@ -1630,10 +1689,10 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G8">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H8">
@@ -1661,7 +1720,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -1678,10 +1737,10 @@
         <v>2</v>
       </c>
       <c r="F9">
-        <v>9.210000000000001</v>
+        <v>9.2100000000000009</v>
       </c>
       <c r="G9">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H9">
@@ -1709,7 +1768,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -1726,10 +1785,10 @@
         <v>2</v>
       </c>
       <c r="F10">
-        <v>9.210000000000001</v>
+        <v>9.2100000000000009</v>
       </c>
       <c r="G10">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H10">
@@ -1738,13 +1797,13 @@
       <c r="I10">
         <v>463</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="1" t="s">
         <v>49</v>
       </c>
       <c r="M10" t="s">
@@ -1757,7 +1816,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -1765,7 +1824,7 @@
         <v>55</v>
       </c>
       <c r="C11">
-        <v>8.841873557642305</v>
+        <v>8.8418735576423053</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
@@ -1774,11 +1833,11 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G11">
-        <f>IF(C:C&gt;F:F,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="H11">
         <v>571</v>
@@ -1805,7 +1864,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1813,7 +1872,7 @@
         <v>61</v>
       </c>
       <c r="C12">
-        <v>6.050891885070516</v>
+        <v>6.0508918850705156</v>
       </c>
       <c r="D12" t="s">
         <v>22</v>
@@ -1822,10 +1881,10 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G12">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H12">
@@ -1853,7 +1912,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -1870,11 +1929,11 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G13">
-        <f>IF(C:C&gt;F:F,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="H13">
         <v>573</v>
@@ -1901,7 +1960,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -1909,7 +1968,7 @@
         <v>73</v>
       </c>
       <c r="C14">
-        <v>5.800050316480865</v>
+        <v>5.8000503164808652</v>
       </c>
       <c r="D14" t="s">
         <v>22</v>
@@ -1918,10 +1977,10 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G14">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H14">
@@ -1949,7 +2008,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>78</v>
       </c>
@@ -1966,11 +2025,11 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G15">
-        <f>IF(C:C&gt;F:F,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="H15">
         <v>576</v>
@@ -1997,7 +2056,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -2014,10 +2073,10 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G16">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H16">
@@ -2045,7 +2104,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>89</v>
       </c>
@@ -2053,7 +2112,7 @@
         <v>90</v>
       </c>
       <c r="C17">
-        <v>1.23679475995117</v>
+        <v>1.2367947599511699</v>
       </c>
       <c r="D17" t="s">
         <v>22</v>
@@ -2062,10 +2121,10 @@
         <v>1</v>
       </c>
       <c r="F17">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G17">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H17">
@@ -2093,7 +2152,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>95</v>
       </c>
@@ -2101,7 +2160,7 @@
         <v>96</v>
       </c>
       <c r="C18">
-        <v>0.3712424378867972</v>
+        <v>0.37124243788679723</v>
       </c>
       <c r="D18" t="s">
         <v>22</v>
@@ -2110,10 +2169,10 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G18">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H18">
@@ -2141,7 +2200,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>101</v>
       </c>
@@ -2149,7 +2208,7 @@
         <v>102</v>
       </c>
       <c r="C19">
-        <v>0.01023926814902453</v>
+        <v>1.023926814902453E-2</v>
       </c>
       <c r="D19" t="s">
         <v>30</v>
@@ -2158,10 +2217,10 @@
         <v>1</v>
       </c>
       <c r="F19">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G19">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H19">
@@ -2189,7 +2248,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>107</v>
       </c>
@@ -2197,7 +2256,7 @@
         <v>108</v>
       </c>
       <c r="C20">
-        <v>9.724844576931527</v>
+        <v>9.7248445769315275</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -2206,11 +2265,11 @@
         <v>1</v>
       </c>
       <c r="F20">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G20">
-        <f>IF(C:C&gt;F:F,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="H20">
         <v>576</v>
@@ -2237,7 +2296,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>113</v>
       </c>
@@ -2245,7 +2304,7 @@
         <v>114</v>
       </c>
       <c r="C21">
-        <v>0.2496721150226313</v>
+        <v>0.24967211502263131</v>
       </c>
       <c r="D21" t="s">
         <v>22</v>
@@ -2254,10 +2313,10 @@
         <v>1</v>
       </c>
       <c r="F21">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G21">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H21">
@@ -2285,7 +2344,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>119</v>
       </c>
@@ -2293,7 +2352,7 @@
         <v>120</v>
       </c>
       <c r="C22">
-        <v>0.00953173397914055</v>
+        <v>9.5317339791405505E-3</v>
       </c>
       <c r="D22" t="s">
         <v>30</v>
@@ -2302,10 +2361,10 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G22">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H22">
@@ -2333,7 +2392,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>125</v>
       </c>
@@ -2341,7 +2400,7 @@
         <v>126</v>
       </c>
       <c r="C23">
-        <v>0.00437624325092353</v>
+        <v>4.3762432509235304E-3</v>
       </c>
       <c r="D23" t="s">
         <v>30</v>
@@ -2350,10 +2409,10 @@
         <v>1</v>
       </c>
       <c r="F23">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G23">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H23">
@@ -2381,7 +2440,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>131</v>
       </c>
@@ -2398,10 +2457,10 @@
         <v>1</v>
       </c>
       <c r="F24">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G24">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H24">
@@ -2429,7 +2488,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -2446,10 +2505,10 @@
         <v>1</v>
       </c>
       <c r="F25">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G25">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H25">
@@ -2477,7 +2536,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>143</v>
       </c>
@@ -2485,7 +2544,7 @@
         <v>144</v>
       </c>
       <c r="C26">
-        <v>0.06473923158126141</v>
+        <v>6.4739231581261408E-2</v>
       </c>
       <c r="D26" t="s">
         <v>30</v>
@@ -2494,10 +2553,10 @@
         <v>1</v>
       </c>
       <c r="F26">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G26">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H26">
@@ -2525,7 +2584,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>149</v>
       </c>
@@ -2533,7 +2592,7 @@
         <v>150</v>
       </c>
       <c r="C27">
-        <v>0.6722442939581668</v>
+        <v>0.67224429395816676</v>
       </c>
       <c r="D27" t="s">
         <v>22</v>
@@ -2542,10 +2601,10 @@
         <v>1</v>
       </c>
       <c r="F27">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G27">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H27">
@@ -2573,7 +2632,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>155</v>
       </c>
@@ -2581,7 +2640,7 @@
         <v>156</v>
       </c>
       <c r="C28">
-        <v>0.00829093652305172</v>
+        <v>8.2909365230517205E-3</v>
       </c>
       <c r="D28" t="s">
         <v>22</v>
@@ -2590,10 +2649,10 @@
         <v>1</v>
       </c>
       <c r="F28">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G28">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H28">
@@ -2621,7 +2680,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>159</v>
       </c>
@@ -2629,7 +2688,7 @@
         <v>160</v>
       </c>
       <c r="C29">
-        <v>70.07804529664047</v>
+        <v>70.078045296640468</v>
       </c>
       <c r="D29" t="s">
         <v>22</v>
@@ -2638,11 +2697,11 @@
         <v>1</v>
       </c>
       <c r="F29">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G29">
-        <f>IF(C:C&gt;F:F,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="H29">
         <v>573</v>
@@ -2669,7 +2728,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>165</v>
       </c>
@@ -2677,7 +2736,7 @@
         <v>166</v>
       </c>
       <c r="C30">
-        <v>27.51712581679149</v>
+        <v>27.517125816791491</v>
       </c>
       <c r="D30" t="s">
         <v>22</v>
@@ -2686,11 +2745,11 @@
         <v>1</v>
       </c>
       <c r="F30">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G30">
-        <f>IF(C:C&gt;F:F,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="H30">
         <v>576</v>
@@ -2717,7 +2776,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>171</v>
       </c>
@@ -2725,7 +2784,7 @@
         <v>172</v>
       </c>
       <c r="C31">
-        <v>2.765632896602101</v>
+        <v>2.7656328966021011</v>
       </c>
       <c r="D31" t="s">
         <v>22</v>
@@ -2734,10 +2793,10 @@
         <v>1</v>
       </c>
       <c r="F31">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G31">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H31">
@@ -2765,7 +2824,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>177</v>
       </c>
@@ -2773,7 +2832,7 @@
         <v>178</v>
       </c>
       <c r="C32">
-        <v>43.10925618375742</v>
+        <v>43.109256183757417</v>
       </c>
       <c r="D32" t="s">
         <v>22</v>
@@ -2782,11 +2841,11 @@
         <v>1</v>
       </c>
       <c r="F32">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G32">
-        <f>IF(C:C&gt;F:F,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="H32">
         <v>574</v>
@@ -2813,7 +2872,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>183</v>
       </c>
@@ -2821,7 +2880,7 @@
         <v>184</v>
       </c>
       <c r="C33">
-        <v>0.6176617628678767</v>
+        <v>0.61766176286787666</v>
       </c>
       <c r="D33" t="s">
         <v>22</v>
@@ -2830,10 +2889,10 @@
         <v>1</v>
       </c>
       <c r="F33">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G33">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H33">
@@ -2861,7 +2920,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>189</v>
       </c>
@@ -2869,7 +2928,7 @@
         <v>190</v>
       </c>
       <c r="C34">
-        <v>23.19392108159503</v>
+        <v>23.193921081595029</v>
       </c>
       <c r="D34" t="s">
         <v>22</v>
@@ -2878,11 +2937,11 @@
         <v>1</v>
       </c>
       <c r="F34">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G34">
-        <f>IF(C:C&gt;F:F,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="H34">
         <v>573</v>
@@ -2909,7 +2968,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>195</v>
       </c>
@@ -2917,7 +2976,7 @@
         <v>196</v>
       </c>
       <c r="C35">
-        <v>0.03176470588235294</v>
+        <v>3.1764705882352938E-2</v>
       </c>
       <c r="D35" t="s">
         <v>22</v>
@@ -2926,10 +2985,10 @@
         <v>1</v>
       </c>
       <c r="F35">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G35">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H35">
@@ -2957,7 +3016,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>201</v>
       </c>
@@ -2965,7 +3024,7 @@
         <v>202</v>
       </c>
       <c r="C36">
-        <v>96.34758342521545</v>
+        <v>96.347583425215447</v>
       </c>
       <c r="D36" t="s">
         <v>22</v>
@@ -2974,11 +3033,11 @@
         <v>1</v>
       </c>
       <c r="F36">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G36">
-        <f>IF(C:C&gt;F:F,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="H36">
         <v>575</v>
@@ -3005,7 +3064,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>207</v>
       </c>
@@ -3013,7 +3072,7 @@
         <v>208</v>
       </c>
       <c r="C37">
-        <v>1.371485859463799</v>
+        <v>1.3714858594637991</v>
       </c>
       <c r="D37" t="s">
         <v>22</v>
@@ -3022,10 +3081,10 @@
         <v>1</v>
       </c>
       <c r="F37">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G37">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" ref="G37:G68" si="1">IF(C:C&gt;F:F,1,0)</f>
         <v>0</v>
       </c>
       <c r="H37">
@@ -3053,7 +3112,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>213</v>
       </c>
@@ -3061,7 +3120,7 @@
         <v>214</v>
       </c>
       <c r="C38">
-        <v>0.3914138236378348</v>
+        <v>0.39141382363783478</v>
       </c>
       <c r="D38" t="s">
         <v>22</v>
@@ -3070,10 +3129,10 @@
         <v>1</v>
       </c>
       <c r="F38">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G38">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H38">
@@ -3101,7 +3160,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>219</v>
       </c>
@@ -3118,10 +3177,10 @@
         <v>1</v>
       </c>
       <c r="F39">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G39">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H39">
@@ -3149,7 +3208,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>225</v>
       </c>
@@ -3157,7 +3216,7 @@
         <v>226</v>
       </c>
       <c r="C40">
-        <v>0.7357900757733749</v>
+        <v>0.73579007577337485</v>
       </c>
       <c r="D40" t="s">
         <v>22</v>
@@ -3166,10 +3225,10 @@
         <v>1</v>
       </c>
       <c r="F40">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G40">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H40">
@@ -3197,7 +3256,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>231</v>
       </c>
@@ -3205,7 +3264,7 @@
         <v>232</v>
       </c>
       <c r="C41">
-        <v>0.9591802247562291</v>
+        <v>0.95918022475622911</v>
       </c>
       <c r="D41" t="s">
         <v>30</v>
@@ -3214,10 +3273,10 @@
         <v>1</v>
       </c>
       <c r="F41">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G41">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H41">
@@ -3245,7 +3304,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>237</v>
       </c>
@@ -3253,7 +3312,7 @@
         <v>238</v>
       </c>
       <c r="C42">
-        <v>1.955947413169174</v>
+        <v>1.9559474131691741</v>
       </c>
       <c r="D42" t="s">
         <v>22</v>
@@ -3262,10 +3321,10 @@
         <v>1</v>
       </c>
       <c r="F42">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G42">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H42">
@@ -3293,7 +3352,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>243</v>
       </c>
@@ -3310,10 +3369,10 @@
         <v>1</v>
       </c>
       <c r="F43">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G43">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H43">
@@ -3341,7 +3400,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>249</v>
       </c>
@@ -3349,7 +3408,7 @@
         <v>250</v>
       </c>
       <c r="C44">
-        <v>1.768152788028401</v>
+        <v>1.7681527880284009</v>
       </c>
       <c r="D44" t="s">
         <v>22</v>
@@ -3358,10 +3417,10 @@
         <v>1</v>
       </c>
       <c r="F44">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G44">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H44">
@@ -3389,7 +3448,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>255</v>
       </c>
@@ -3406,10 +3465,10 @@
         <v>1</v>
       </c>
       <c r="F45">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G45">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H45">
@@ -3437,7 +3496,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>261</v>
       </c>
@@ -3454,10 +3513,10 @@
         <v>1</v>
       </c>
       <c r="F46">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G46">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H46">
@@ -3485,7 +3544,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>267</v>
       </c>
@@ -3502,10 +3561,10 @@
         <v>1</v>
       </c>
       <c r="F47">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G47">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H47">
@@ -3533,7 +3592,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>273</v>
       </c>
@@ -3541,7 +3600,7 @@
         <v>274</v>
       </c>
       <c r="C48">
-        <v>1.144451283400376</v>
+        <v>1.1444512834003759</v>
       </c>
       <c r="D48" t="s">
         <v>22</v>
@@ -3550,10 +3609,10 @@
         <v>1</v>
       </c>
       <c r="F48">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G48">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H48">
@@ -3581,7 +3640,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>279</v>
       </c>
@@ -3589,7 +3648,7 @@
         <v>280</v>
       </c>
       <c r="C49">
-        <v>0.0489892031301854</v>
+        <v>4.8989203130185399E-2</v>
       </c>
       <c r="D49" t="s">
         <v>22</v>
@@ -3598,10 +3657,10 @@
         <v>1</v>
       </c>
       <c r="F49">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G49">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H49">
@@ -3629,7 +3688,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>285</v>
       </c>
@@ -3637,7 +3696,7 @@
         <v>286</v>
       </c>
       <c r="C50">
-        <v>0.1753027564685551</v>
+        <v>0.17530275646855509</v>
       </c>
       <c r="D50" t="s">
         <v>22</v>
@@ -3646,10 +3705,10 @@
         <v>1</v>
       </c>
       <c r="F50">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G50">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H50">
@@ -3677,7 +3736,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>291</v>
       </c>
@@ -3685,7 +3744,7 @@
         <v>292</v>
       </c>
       <c r="C51">
-        <v>0.8730331979740995</v>
+        <v>0.87303319797409951</v>
       </c>
       <c r="D51" t="s">
         <v>22</v>
@@ -3694,10 +3753,10 @@
         <v>1</v>
       </c>
       <c r="F51">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G51">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H51">
@@ -3725,7 +3784,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>297</v>
       </c>
@@ -3733,7 +3792,7 @@
         <v>298</v>
       </c>
       <c r="C52">
-        <v>0.5535950046442071</v>
+        <v>0.55359500464420708</v>
       </c>
       <c r="D52" t="s">
         <v>22</v>
@@ -3742,10 +3801,10 @@
         <v>1</v>
       </c>
       <c r="F52">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G52">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H52">
@@ -3773,7 +3832,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>303</v>
       </c>
@@ -3781,7 +3840,7 @@
         <v>304</v>
       </c>
       <c r="C53">
-        <v>2.846860097160935</v>
+        <v>2.8468600971609348</v>
       </c>
       <c r="D53" t="s">
         <v>22</v>
@@ -3790,10 +3849,10 @@
         <v>1</v>
       </c>
       <c r="F53">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G53">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H53">
@@ -3821,7 +3880,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -3829,7 +3888,7 @@
         <v>309</v>
       </c>
       <c r="C54">
-        <v>0.08484712480947734</v>
+        <v>8.4847124809477342E-2</v>
       </c>
       <c r="D54" t="s">
         <v>22</v>
@@ -3838,10 +3897,10 @@
         <v>1</v>
       </c>
       <c r="F54">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G54">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H54">
@@ -3869,7 +3928,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>13</v>
       </c>
@@ -3877,7 +3936,7 @@
         <v>314</v>
       </c>
       <c r="C55">
-        <v>0.4830997914640373</v>
+        <v>0.48309979146403731</v>
       </c>
       <c r="D55" t="s">
         <v>22</v>
@@ -3886,10 +3945,10 @@
         <v>1</v>
       </c>
       <c r="F55">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G55">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H55">
@@ -3917,7 +3976,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>319</v>
       </c>
@@ -3925,7 +3984,7 @@
         <v>320</v>
       </c>
       <c r="C56">
-        <v>0.003054411962186961</v>
+        <v>3.0544119621869611E-3</v>
       </c>
       <c r="D56" t="s">
         <v>22</v>
@@ -3934,10 +3993,10 @@
         <v>1</v>
       </c>
       <c r="F56">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G56">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H56">
@@ -3965,7 +4024,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>325</v>
       </c>
@@ -3982,10 +4041,10 @@
         <v>1</v>
       </c>
       <c r="F57">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G57">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H57">
@@ -4013,7 +4072,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>331</v>
       </c>
@@ -4021,7 +4080,7 @@
         <v>332</v>
       </c>
       <c r="C58">
-        <v>0.464360289590138</v>
+        <v>0.46436028959013798</v>
       </c>
       <c r="D58" t="s">
         <v>22</v>
@@ -4030,10 +4089,10 @@
         <v>1</v>
       </c>
       <c r="F58">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G58">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H58">
@@ -4061,7 +4120,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>337</v>
       </c>
@@ -4069,7 +4128,7 @@
         <v>338</v>
       </c>
       <c r="C59">
-        <v>0.5609866414528766</v>
+        <v>0.56098664145287658</v>
       </c>
       <c r="D59" t="s">
         <v>22</v>
@@ -4078,10 +4137,10 @@
         <v>1</v>
       </c>
       <c r="F59">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G59">
-        <f>IF(C:C&gt;F:F,1,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H59">
@@ -4109,7 +4168,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>343</v>
       </c>
@@ -4117,7 +4176,7 @@
         <v>344</v>
       </c>
       <c r="C60">
-        <v>7.334161031342555</v>
+        <v>7.3341610313425551</v>
       </c>
       <c r="D60" t="s">
         <v>22</v>
@@ -4126,11 +4185,11 @@
         <v>1</v>
       </c>
       <c r="F60">
-        <v>6.635</v>
+        <v>6.6349999999999998</v>
       </c>
       <c r="G60">
-        <f>IF(C:C&gt;F:F,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="H60">
         <v>566</v>

</xml_diff>